<commit_message>
Starting work on events for logic
</commit_message>
<xml_diff>
--- a/TODO_List.xlsx
+++ b/TODO_List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\clash\CourseWork\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BE6EB45-0594-404A-9775-D5F6C23D1E6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{105DF32D-9428-422C-A780-BD3D22B65A5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15270" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -61,13 +61,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC000"/>
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0"/>
+        <fgColor rgb="FF00B050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -390,7 +390,7 @@
   <dimension ref="G11:H15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L14" sqref="L14"/>
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -410,21 +410,21 @@
       <c r="G12" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="H12" s="3"/>
+      <c r="H12" s="4"/>
     </row>
     <row r="13" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G13" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="H13" s="3"/>
+      <c r="H13" s="4"/>
     </row>
     <row r="14" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G14" s="1"/>
-      <c r="H14" s="4"/>
+      <c r="H14" s="3"/>
     </row>
     <row r="15" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G15" s="1"/>
-      <c r="H15" s="4"/>
+      <c r="H15" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>